<commit_message>
Altera modelo de dados spmedgroup
</commit_message>
<xml_diff>
--- a/apoio/modelos/sp_med_group/dados_spmedgroup.xlsx
+++ b/apoio/modelos/sp_med_group/dados_spmedgroup.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20354"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20371"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adminlocal\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saulo.santos\Downloads\SENAI\CT\2021-1S-2D\senai-dev-1s2021-alunos\apoio\modelos\sp_med_group\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E771BDDF-C71C-485E-B6ED-369D51E9E5E1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A802AF8-638E-4C1D-A1CA-49CFAF0709A2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7860" windowHeight="7464" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5640" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Especialidades" sheetId="2" r:id="rId1"/>
@@ -258,9 +258,6 @@
     <t>54366362-5</t>
   </si>
   <si>
-    <t>t32544444-1</t>
-  </si>
-  <si>
     <t>54566266-7</t>
   </si>
   <si>
@@ -280,6 +277,9 @@
   </si>
   <si>
     <t>65463-SP</t>
+  </si>
+  <si>
+    <t>53254444-1</t>
   </si>
 </sst>
 </file>
@@ -681,13 +681,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="A18" sqref="A2:A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.88671875" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
@@ -789,20 +789,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="35.21875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="10.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.44140625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="36.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="16384" width="19.6640625" style="2"/>
   </cols>
   <sheetData>
@@ -820,7 +820,7 @@
         <v>21</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>22</v>
@@ -834,7 +834,7 @@
     </row>
     <row r="2" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>15</v>
@@ -860,7 +860,7 @@
     </row>
     <row r="3" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>16</v>
@@ -886,13 +886,13 @@
     </row>
     <row r="4" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>32</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>28</v>
@@ -924,13 +924,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="23.44140625" style="3"/>
+    <col min="1" max="1" width="10.21875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="19.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.109375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="14.88671875" style="3" customWidth="1"/>
+    <col min="7" max="7" width="66.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="23.44140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -1062,7 +1069,7 @@
         <v>55</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="F6" s="3">
         <v>91305348010</v>
@@ -1085,7 +1092,7 @@
         <v>59</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F7" s="3">
         <v>79799299004</v>
@@ -1105,7 +1112,7 @@
         <v>43164</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F8" s="3">
         <v>13771913039</v>
@@ -1132,16 +1139,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.33203125" style="12" customWidth="1"/>
-    <col min="4" max="4" width="14.109375" style="3" customWidth="1"/>
+    <col min="1" max="1" width="9.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>

</xml_diff>